<commit_message>
Change data for test purpose
</commit_message>
<xml_diff>
--- a/Python/HEL/data/Drones_Params.xlsx
+++ b/Python/HEL/data/Drones_Params.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\GITHUB_REPOSITORIES\Sandbox\Python\HEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612FF11-C566-4A62-920C-768C88B44FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8DDFBE-4661-4A40-BF81-3D1685912B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,7 +500,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>12.3</v>
+        <v>112.3</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -522,13 +522,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -551,7 +551,7 @@
         <v>12.3</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="C2">
         <v>0.15</v>

</xml_diff>

<commit_message>
Put useful names for the different drones
</commit_message>
<xml_diff>
--- a/Python/HEL/data/Drones_Params.xlsx
+++ b/Python/HEL/data/Drones_Params.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\GITHUB_REPOSITORIES\Sandbox\Python\HEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8DDFBE-4661-4A40-BF81-3D1685912B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193F7129-3855-41F5-8E29-F2A8A82E89B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{66D518BA-4A41-414E-B35F-9020CADD6206}"/>
   </bookViews>
   <sheets>
-    <sheet name="DRONE1" sheetId="3" r:id="rId1"/>
-    <sheet name="DRONE2" sheetId="4" r:id="rId2"/>
-    <sheet name="DRONE3" sheetId="5" r:id="rId3"/>
+    <sheet name="DRONES" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Damage Fluence</t>
   </si>
@@ -48,6 +46,18 @@
   </si>
   <si>
     <t>Lz</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DJI Phantom 4</t>
+  </si>
+  <si>
+    <t>DJI Mavic 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Custom Drone 1</t>
   </si>
 </sst>
 </file>
@@ -405,53 +415,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B98EE9-1508-4B16-AF2C-76E84B48B1FF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>12.3</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.15</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>25.6</v>
+      </c>
+      <c r="C3">
+        <v>0.15</v>
+      </c>
+      <c r="D3">
+        <v>0.98</v>
+      </c>
+      <c r="E3">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="C4">
+        <v>0.23</v>
+      </c>
+      <c r="D4">
+        <v>0.17</v>
+      </c>
+      <c r="E4">
+        <v>0.57999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -459,108 +510,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD74123E-0597-4BAA-AA7D-F1AE792A159A}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>112.3</v>
-      </c>
-      <c r="B2">
-        <v>0.5</v>
-      </c>
-      <c r="C2">
-        <v>0.15</v>
-      </c>
-      <c r="D2">
-        <v>0.26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B7709-702B-4F54-A3B5-835BBDA57EA2}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>12.3</v>
-      </c>
-      <c r="B2">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="C2">
-        <v>0.15</v>
-      </c>
-      <c r="D2">
-        <v>0.26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>